<commit_message>
v0.56 Add Mixer control
1. Add Mixer control
2. Add Noise Gate
</commit_message>
<xml_diff>
--- a/Documentation/Feedback & ToDoList/4711_GUI_FB_1.1.xlsx
+++ b/Documentation/Feedback & ToDoList/4711_GUI_FB_1.1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="193">
   <si>
     <t>I2C Device Address加上</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -940,6 +940,10 @@
   </si>
   <si>
     <t>Fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1070,7 +1074,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1135,6 +1139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="差" xfId="3" builtinId="27"/>
@@ -1175,7 +1180,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1375A446-59C3-4408-9B54-31A206487CDA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1375A446-59C3-4408-9B54-31A206487CDA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1219,7 +1224,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C10189AD-A3A4-4692-9AD8-ED27FA1AD856}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C10189AD-A3A4-4692-9AD8-ED27FA1AD856}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1263,7 +1268,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5458403-52AE-49CF-B170-B077049CF2C4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5458403-52AE-49CF-B170-B077049CF2C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1995,10 +2000,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H115"/>
+  <dimension ref="B2:J115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="H113" sqref="H113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2375,7 +2380,7 @@
       </c>
     </row>
     <row r="42" spans="4:8" ht="24" customHeight="1">
-      <c r="E42" s="39">
+      <c r="E42" s="40">
         <v>2</v>
       </c>
       <c r="F42" s="9" t="s">
@@ -2383,7 +2388,7 @@
       </c>
     </row>
     <row r="43" spans="4:8" ht="108">
-      <c r="E43" s="39"/>
+      <c r="E43" s="40"/>
       <c r="F43" s="14" t="s">
         <v>98</v>
       </c>
@@ -2716,7 +2721,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="4:8" s="28" customFormat="1">
+    <row r="81" spans="4:10" s="28" customFormat="1">
       <c r="D81" s="12"/>
       <c r="E81" s="9">
         <v>5</v>
@@ -2728,7 +2733,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="4:8" s="33" customFormat="1">
+    <row r="82" spans="4:10" s="33" customFormat="1">
       <c r="D82" s="12"/>
       <c r="E82" s="12">
         <v>6</v>
@@ -2740,7 +2745,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="83" spans="4:8" s="33" customFormat="1">
+    <row r="83" spans="4:10" s="33" customFormat="1">
       <c r="D83" s="12"/>
       <c r="E83" s="12">
         <v>7</v>
@@ -2752,7 +2757,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="4:8" s="33" customFormat="1">
+    <row r="84" spans="4:10" s="33" customFormat="1">
       <c r="D84" s="12"/>
       <c r="E84" s="12">
         <v>8</v>
@@ -2764,7 +2769,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="85" spans="4:8" s="34" customFormat="1">
+    <row r="85" spans="4:10" s="34" customFormat="1">
       <c r="D85" s="12"/>
       <c r="E85" s="12">
         <v>9</v>
@@ -2777,7 +2782,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="86" spans="4:8" s="36" customFormat="1">
+    <row r="86" spans="4:10" s="36" customFormat="1">
       <c r="D86" s="12"/>
       <c r="E86" s="12">
         <v>10</v>
@@ -2789,7 +2794,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="87" spans="4:8" s="36" customFormat="1">
+    <row r="87" spans="4:10" s="36" customFormat="1">
       <c r="D87" s="12"/>
       <c r="E87" s="12">
         <v>11</v>
@@ -2801,7 +2806,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="4:8" s="37" customFormat="1">
+    <row r="88" spans="4:10" s="37" customFormat="1">
       <c r="D88" s="12"/>
       <c r="E88" s="12">
         <v>12</v>
@@ -2813,7 +2818,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="90" spans="4:8">
+    <row r="90" spans="4:10">
       <c r="D90" s="10" t="s">
         <v>77</v>
       </c>
@@ -2824,8 +2829,11 @@
       <c r="G90" s="26" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="92" spans="4:8">
+      <c r="J90" s="39" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="92" spans="4:10">
       <c r="D92" s="9" t="s">
         <v>79</v>
       </c>
@@ -2836,7 +2844,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="93" spans="4:8" s="15" customFormat="1">
+    <row r="93" spans="4:10" s="15" customFormat="1">
       <c r="E93" s="15">
         <v>2</v>
       </c>
@@ -2847,7 +2855,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="95" spans="4:8">
+    <row r="95" spans="4:10">
       <c r="D95" s="9" t="s">
         <v>80</v>
       </c>
@@ -2858,7 +2866,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="4:8">
+    <row r="96" spans="4:10">
       <c r="D96" s="9"/>
       <c r="E96" s="9">
         <v>2</v>
@@ -2939,11 +2947,17 @@
       <c r="G103" s="26" t="s">
         <v>148</v>
       </c>
+      <c r="H103" s="10" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="104" spans="4:8">
       <c r="D104" s="10"/>
       <c r="E104" s="10"/>
       <c r="F104" s="10"/>
+      <c r="H104" s="39" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="105" spans="4:8" ht="27">
       <c r="D105" s="10" t="s">
@@ -2956,6 +2970,9 @@
       <c r="G105" s="26" t="s">
         <v>149</v>
       </c>
+      <c r="H105" s="39" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="107" spans="4:8">
       <c r="D107" s="19" t="s">
@@ -3011,6 +3028,9 @@
       </c>
       <c r="G112" s="26" t="s">
         <v>150</v>
+      </c>
+      <c r="H112" s="10" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="115" spans="2:6">

</xml_diff>